<commit_message>
Changed Excel File and added something
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Tutorial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9828C5D4-9D07-4811-B0FC-CB6B1EAB6B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CFD58A-308D-478A-B598-EE6DF828B46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,32 +337,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="U2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I3">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="J6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>